<commit_message>
fix(): Salesforce mandatory fields
</commit_message>
<xml_diff>
--- a/default-mappings-xlsx/grabber/Grabber_Mapping_Salesforce_DE.xlsx
+++ b/default-mappings-xlsx/grabber/Grabber_Mapping_Salesforce_DE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ValentinSchönrock\Documents\GitRepos\snapaddy-faq-attachments\default-mappings-xlsx\grabber\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479056EC-2D41-43D4-BB93-17BF69BA241D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB71EE8-B922-4830-B338-8F8B1EEAADBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2250" windowWidth="11370" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specifications" sheetId="2" r:id="rId1"/>
@@ -363,7 +363,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="70">
+  <borders count="68">
     <border>
       <left/>
       <right/>
@@ -831,21 +831,6 @@
       <right style="thin">
         <color rgb="FF9DA600"/>
       </right>
-      <top style="thick">
-        <color rgb="FF9DA600"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF9DA600"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF9DA600"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF9DA600"/>
-      </right>
       <top style="thin">
         <color rgb="FF9DA600"/>
       </top>
@@ -977,19 +962,6 @@
       <bottom style="thick">
         <color rgb="FF9DA600"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF9DA600"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF9DA600"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF9DA600"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1250,7 +1222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1295,25 +1267,25 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1331,7 +1303,7 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1341,18 +1313,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1363,60 +1329,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="59" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="62" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="61" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="60" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="64" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="63" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="62" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1435,11 +1377,472 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="71">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike/>
+        <color rgb="FFFE6C36"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkDown">
+          <fgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FF9DA600"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1800,11 +2203,11 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="snapADDY" pivot="0" count="5" xr9:uid="{A8851A67-88BF-475D-B211-A3CFCBFE5DEE}">
-      <tableStyleElement type="wholeTable" dxfId="30"/>
-      <tableStyleElement type="headerRow" dxfId="29"/>
-      <tableStyleElement type="firstColumn" dxfId="28"/>
-      <tableStyleElement type="firstRowStripe" dxfId="27"/>
-      <tableStyleElement type="secondRowStripe" dxfId="26"/>
+      <tableStyleElement type="wholeTable" dxfId="70"/>
+      <tableStyleElement type="headerRow" dxfId="69"/>
+      <tableStyleElement type="firstColumn" dxfId="68"/>
+      <tableStyleElement type="firstRowStripe" dxfId="67"/>
+      <tableStyleElement type="secondRowStripe" dxfId="66"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2279,7 +2682,7 @@
   <dimension ref="A1:Y36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2328,44 +2731,44 @@
         <v>66</v>
       </c>
       <c r="E3" s="35"/>
-      <c r="G3" s="96" t="s">
+      <c r="G3" s="102" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
+      <c r="H3" s="102"/>
+      <c r="I3" s="102"/>
       <c r="J3" s="5"/>
-      <c r="K3" s="96" t="s">
+      <c r="K3" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="O3" s="96" t="s">
+      <c r="L3" s="102"/>
+      <c r="M3" s="102"/>
+      <c r="O3" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="P3" s="96"/>
-      <c r="Q3" s="96"/>
-      <c r="S3" s="93" t="s">
+      <c r="P3" s="102"/>
+      <c r="Q3" s="102"/>
+      <c r="S3" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="T3" s="94"/>
-      <c r="U3" s="95"/>
-      <c r="W3" s="93" t="s">
+      <c r="T3" s="100"/>
+      <c r="U3" s="101"/>
+      <c r="W3" s="99" t="s">
         <v>65</v>
       </c>
-      <c r="X3" s="94"/>
-      <c r="Y3" s="95"/>
+      <c r="X3" s="100"/>
+      <c r="Y3" s="101"/>
     </row>
     <row r="4" spans="1:25" ht="7.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:25" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="72" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="56" t="s">
         <v>73</v>
       </c>
       <c r="C5" s="57"/>
-      <c r="D5" s="76"/>
-      <c r="E5" s="77" t="s">
+      <c r="D5" s="73"/>
+      <c r="E5" s="74" t="s">
         <v>37</v>
       </c>
       <c r="G5" s="17" t="s">
@@ -2396,27 +2799,27 @@
       <c r="Q5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="S5" s="78" t="s">
+      <c r="S5" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="T5" s="79" t="s">
+      <c r="T5" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="U5" s="80" t="s">
+      <c r="U5" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="W5" s="78" t="s">
+      <c r="W5" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="X5" s="79" t="s">
+      <c r="X5" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="Y5" s="80" t="s">
+      <c r="Y5" s="77" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="74"/>
+      <c r="A6" s="71"/>
       <c r="B6" s="24"/>
       <c r="C6" s="58"/>
       <c r="D6" s="29"/>
@@ -2431,23 +2834,23 @@
       <c r="O6" s="15"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="16"/>
-      <c r="S6" s="81" t="s">
+      <c r="S6" s="78" t="s">
         <v>31</v>
       </c>
       <c r="T6" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="U6" s="82"/>
-      <c r="W6" s="88"/>
+      <c r="U6" s="79"/>
+      <c r="W6" s="85"/>
       <c r="X6" s="4"/>
-      <c r="Y6" s="89"/>
+      <c r="Y6" s="86"/>
     </row>
     <row r="7" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="65" t="s">
+      <c r="A7" s="63" t="s">
         <v>39</v>
       </c>
       <c r="B7" s="46"/>
-      <c r="C7" s="59"/>
+      <c r="C7" s="58"/>
       <c r="D7" s="47"/>
       <c r="E7" s="48"/>
       <c r="G7" s="49" t="s">
@@ -2472,23 +2875,23 @@
       <c r="O7" s="53"/>
       <c r="P7" s="54"/>
       <c r="Q7" s="55"/>
-      <c r="S7" s="83" t="s">
+      <c r="S7" s="80" t="s">
         <v>33</v>
       </c>
       <c r="T7" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="U7" s="82"/>
-      <c r="W7" s="84"/>
+      <c r="U7" s="79"/>
+      <c r="W7" s="81"/>
       <c r="X7" s="3"/>
-      <c r="Y7" s="82"/>
+      <c r="Y7" s="79"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A8" s="66" t="s">
+      <c r="A8" s="64" t="s">
         <v>40</v>
       </c>
       <c r="B8" s="25"/>
-      <c r="C8" s="60"/>
+      <c r="C8" s="58"/>
       <c r="D8" s="30"/>
       <c r="E8" s="39"/>
       <c r="G8" s="8" t="s">
@@ -2513,19 +2916,19 @@
       <c r="O8" s="8"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="9"/>
-      <c r="S8" s="84"/>
+      <c r="S8" s="81"/>
       <c r="T8" s="3"/>
-      <c r="U8" s="82"/>
-      <c r="W8" s="84"/>
+      <c r="U8" s="79"/>
+      <c r="W8" s="81"/>
       <c r="X8" s="3"/>
-      <c r="Y8" s="82"/>
+      <c r="Y8" s="79"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A9" s="66" t="s">
+      <c r="A9" s="64" t="s">
         <v>41</v>
       </c>
       <c r="B9" s="25"/>
-      <c r="C9" s="60"/>
+      <c r="C9" s="58"/>
       <c r="D9" s="30"/>
       <c r="E9" s="39"/>
       <c r="G9" s="8" t="s">
@@ -2550,19 +2953,19 @@
       <c r="O9" s="8"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="9"/>
-      <c r="S9" s="84"/>
+      <c r="S9" s="81"/>
       <c r="T9" s="3"/>
-      <c r="U9" s="82"/>
-      <c r="W9" s="84"/>
+      <c r="U9" s="79"/>
+      <c r="W9" s="81"/>
       <c r="X9" s="3"/>
-      <c r="Y9" s="82"/>
+      <c r="Y9" s="79"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A10" s="66" t="s">
+      <c r="A10" s="64" t="s">
         <v>42</v>
       </c>
       <c r="B10" s="25"/>
-      <c r="C10" s="60"/>
+      <c r="C10" s="58"/>
       <c r="D10" s="30"/>
       <c r="E10" s="39"/>
       <c r="G10" s="8" t="s">
@@ -2587,19 +2990,19 @@
       <c r="O10" s="8"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="9"/>
-      <c r="S10" s="81"/>
+      <c r="S10" s="78"/>
       <c r="T10" s="50"/>
-      <c r="U10" s="85"/>
-      <c r="W10" s="84"/>
+      <c r="U10" s="82"/>
+      <c r="W10" s="81"/>
       <c r="X10" s="3"/>
-      <c r="Y10" s="82"/>
+      <c r="Y10" s="79"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A11" s="66" t="s">
+      <c r="A11" s="64" t="s">
         <v>43</v>
       </c>
       <c r="B11" s="25"/>
-      <c r="C11" s="60"/>
+      <c r="C11" s="58"/>
       <c r="D11" s="30"/>
       <c r="E11" s="39"/>
       <c r="G11" s="8" t="s">
@@ -2624,19 +3027,19 @@
       <c r="Q11" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="S11" s="84"/>
+      <c r="S11" s="81"/>
       <c r="T11" s="3"/>
-      <c r="U11" s="82"/>
-      <c r="W11" s="84"/>
+      <c r="U11" s="79"/>
+      <c r="W11" s="81"/>
       <c r="X11" s="3"/>
-      <c r="Y11" s="82"/>
+      <c r="Y11" s="79"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A12" s="67" t="s">
+      <c r="A12" s="65" t="s">
         <v>46</v>
       </c>
       <c r="B12" s="26"/>
-      <c r="C12" s="60"/>
+      <c r="C12" s="58"/>
       <c r="D12" s="30"/>
       <c r="E12" s="39"/>
       <c r="G12" s="15" t="s">
@@ -2667,19 +3070,19 @@
       <c r="Q12" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="S12" s="86"/>
+      <c r="S12" s="83"/>
       <c r="T12" s="54"/>
-      <c r="U12" s="87"/>
-      <c r="W12" s="84"/>
+      <c r="U12" s="84"/>
+      <c r="W12" s="81"/>
       <c r="X12" s="3"/>
-      <c r="Y12" s="82"/>
+      <c r="Y12" s="79"/>
     </row>
     <row r="13" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="65" t="s">
+      <c r="A13" s="63" t="s">
         <v>47</v>
       </c>
       <c r="B13" s="46"/>
-      <c r="C13" s="59"/>
+      <c r="C13" s="58"/>
       <c r="D13" s="47"/>
       <c r="E13" s="48"/>
       <c r="G13" s="53" t="s">
@@ -2710,19 +3113,19 @@
       <c r="Q13" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="S13" s="81"/>
+      <c r="S13" s="78"/>
       <c r="T13" s="50"/>
-      <c r="U13" s="85"/>
-      <c r="W13" s="86"/>
+      <c r="U13" s="82"/>
+      <c r="W13" s="83"/>
       <c r="X13" s="54"/>
-      <c r="Y13" s="87"/>
+      <c r="Y13" s="84"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14" s="68" t="s">
+      <c r="A14" s="66" t="s">
         <v>50</v>
       </c>
       <c r="B14" s="27"/>
-      <c r="C14" s="60"/>
+      <c r="C14" s="58"/>
       <c r="D14" s="30"/>
       <c r="E14" s="39"/>
       <c r="G14" s="13" t="s">
@@ -2753,19 +3156,19 @@
       <c r="Q14" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="S14" s="83"/>
+      <c r="S14" s="80"/>
       <c r="T14" s="14"/>
-      <c r="U14" s="82"/>
-      <c r="W14" s="84"/>
+      <c r="U14" s="79"/>
+      <c r="W14" s="81"/>
       <c r="X14" s="3"/>
-      <c r="Y14" s="82"/>
+      <c r="Y14" s="79"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A15" s="66" t="s">
+      <c r="A15" s="64" t="s">
         <v>48</v>
       </c>
       <c r="B15" s="25"/>
-      <c r="C15" s="60"/>
+      <c r="C15" s="58"/>
       <c r="D15" s="30"/>
       <c r="E15" s="39"/>
       <c r="G15" s="8" t="s">
@@ -2796,19 +3199,19 @@
       <c r="Q15" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="S15" s="84"/>
+      <c r="S15" s="81"/>
       <c r="T15" s="3"/>
-      <c r="U15" s="82"/>
-      <c r="W15" s="84"/>
+      <c r="U15" s="79"/>
+      <c r="W15" s="81"/>
       <c r="X15" s="3"/>
-      <c r="Y15" s="82"/>
+      <c r="Y15" s="79"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A16" s="66" t="s">
+      <c r="A16" s="64" t="s">
         <v>49</v>
       </c>
       <c r="B16" s="25"/>
-      <c r="C16" s="60"/>
+      <c r="C16" s="58"/>
       <c r="D16" s="30"/>
       <c r="E16" s="39"/>
       <c r="G16" s="8" t="s">
@@ -2839,19 +3242,19 @@
       <c r="Q16" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="S16" s="84"/>
+      <c r="S16" s="81"/>
       <c r="T16" s="3"/>
-      <c r="U16" s="82"/>
-      <c r="W16" s="84"/>
+      <c r="U16" s="79"/>
+      <c r="W16" s="81"/>
       <c r="X16" s="3"/>
-      <c r="Y16" s="82"/>
+      <c r="Y16" s="79"/>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A17" s="66" t="s">
+      <c r="A17" s="64" t="s">
         <v>44</v>
       </c>
       <c r="B17" s="25"/>
-      <c r="C17" s="60"/>
+      <c r="C17" s="58"/>
       <c r="D17" s="30"/>
       <c r="E17" s="39"/>
       <c r="G17" s="8" t="s">
@@ -2882,19 +3285,19 @@
       <c r="Q17" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="S17" s="84"/>
+      <c r="S17" s="81"/>
       <c r="T17" s="3"/>
-      <c r="U17" s="82"/>
-      <c r="W17" s="84"/>
+      <c r="U17" s="79"/>
+      <c r="W17" s="81"/>
       <c r="X17" s="3"/>
-      <c r="Y17" s="82"/>
+      <c r="Y17" s="79"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A18" s="66" t="s">
+      <c r="A18" s="64" t="s">
         <v>45</v>
       </c>
       <c r="B18" s="25"/>
-      <c r="C18" s="60"/>
+      <c r="C18" s="58"/>
       <c r="D18" s="30"/>
       <c r="E18" s="39"/>
       <c r="G18" s="8" t="s">
@@ -2919,19 +3322,19 @@
       <c r="O18" s="8"/>
       <c r="P18" s="3"/>
       <c r="Q18" s="9"/>
-      <c r="S18" s="84"/>
+      <c r="S18" s="81"/>
       <c r="T18" s="3"/>
-      <c r="U18" s="82"/>
-      <c r="W18" s="84"/>
+      <c r="U18" s="79"/>
+      <c r="W18" s="81"/>
       <c r="X18" s="3"/>
-      <c r="Y18" s="82"/>
+      <c r="Y18" s="79"/>
     </row>
     <row r="19" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="65" t="s">
+      <c r="A19" s="63" t="s">
         <v>2</v>
       </c>
       <c r="B19" s="46"/>
-      <c r="C19" s="59"/>
+      <c r="C19" s="58"/>
       <c r="D19" s="47"/>
       <c r="E19" s="48"/>
       <c r="G19" s="53" t="s">
@@ -2962,19 +3365,19 @@
       <c r="Q19" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="S19" s="86"/>
+      <c r="S19" s="83"/>
       <c r="T19" s="54"/>
-      <c r="U19" s="87"/>
-      <c r="W19" s="86"/>
+      <c r="U19" s="84"/>
+      <c r="W19" s="83"/>
       <c r="X19" s="54"/>
-      <c r="Y19" s="87"/>
+      <c r="Y19" s="84"/>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A20" s="66" t="s">
+      <c r="A20" s="64" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="25"/>
-      <c r="C20" s="60"/>
+      <c r="C20" s="58"/>
       <c r="D20" s="30"/>
       <c r="E20" s="39"/>
       <c r="G20" s="8" t="s">
@@ -2999,19 +3402,19 @@
       <c r="O20" s="8"/>
       <c r="P20" s="3"/>
       <c r="Q20" s="9"/>
-      <c r="S20" s="84"/>
+      <c r="S20" s="81"/>
       <c r="T20" s="3"/>
-      <c r="U20" s="82"/>
-      <c r="W20" s="84"/>
+      <c r="U20" s="79"/>
+      <c r="W20" s="81"/>
       <c r="X20" s="3"/>
-      <c r="Y20" s="82"/>
+      <c r="Y20" s="79"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A21" s="67" t="s">
+      <c r="A21" s="65" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="25"/>
-      <c r="C21" s="60"/>
+      <c r="C21" s="58"/>
       <c r="D21" s="30"/>
       <c r="E21" s="39"/>
       <c r="G21" s="15" t="s">
@@ -3036,19 +3439,19 @@
       <c r="Q21" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="S21" s="88"/>
+      <c r="S21" s="85"/>
       <c r="T21" s="4"/>
-      <c r="U21" s="89"/>
-      <c r="W21" s="88"/>
+      <c r="U21" s="86"/>
+      <c r="W21" s="85"/>
       <c r="X21" s="4"/>
-      <c r="Y21" s="89"/>
+      <c r="Y21" s="86"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A22" s="67" t="s">
+      <c r="A22" s="65" t="s">
         <v>55</v>
       </c>
       <c r="B22" s="25"/>
-      <c r="C22" s="60"/>
+      <c r="C22" s="58"/>
       <c r="D22" s="30"/>
       <c r="E22" s="39"/>
       <c r="G22" s="15" t="s">
@@ -3067,21 +3470,21 @@
       <c r="O22" s="15"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="9"/>
-      <c r="S22" s="88"/>
+      <c r="S22" s="85"/>
       <c r="T22" s="4"/>
-      <c r="U22" s="89"/>
-      <c r="W22" s="88"/>
+      <c r="U22" s="86"/>
+      <c r="W22" s="85"/>
       <c r="X22" s="4"/>
-      <c r="Y22" s="89"/>
+      <c r="Y22" s="86"/>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A23" s="67" t="s">
+      <c r="A23" s="65" t="s">
         <v>56</v>
       </c>
       <c r="B23" s="26"/>
-      <c r="C23" s="70"/>
-      <c r="D23" s="71"/>
-      <c r="E23" s="72"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="69"/>
       <c r="G23" s="15" t="s">
         <v>56</v>
       </c>
@@ -3098,19 +3501,19 @@
       <c r="O23" s="15"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="9"/>
-      <c r="S23" s="88"/>
+      <c r="S23" s="85"/>
       <c r="T23" s="4"/>
-      <c r="U23" s="89"/>
-      <c r="W23" s="88"/>
+      <c r="U23" s="86"/>
+      <c r="W23" s="85"/>
       <c r="X23" s="4"/>
-      <c r="Y23" s="89"/>
+      <c r="Y23" s="86"/>
     </row>
     <row r="24" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="21" t="s">
         <v>57</v>
       </c>
       <c r="B24" s="28"/>
-      <c r="C24" s="61"/>
+      <c r="C24" s="59"/>
       <c r="D24" s="31"/>
       <c r="E24" s="40"/>
       <c r="G24" s="10" t="s">
@@ -3141,12 +3544,12 @@
       <c r="Q24" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="S24" s="90"/>
-      <c r="T24" s="91"/>
-      <c r="U24" s="92"/>
-      <c r="W24" s="90"/>
-      <c r="X24" s="91"/>
-      <c r="Y24" s="92"/>
+      <c r="S24" s="87"/>
+      <c r="T24" s="88"/>
+      <c r="U24" s="89"/>
+      <c r="W24" s="87"/>
+      <c r="X24" s="88"/>
+      <c r="Y24" s="89"/>
     </row>
     <row r="25" spans="1:25" ht="7.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G25" s="6"/>
@@ -3159,16 +3562,16 @@
       <c r="O25" s="6"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="7"/>
-      <c r="S25" s="62"/>
+      <c r="S25" s="60"/>
       <c r="T25" s="2"/>
-      <c r="U25" s="63"/>
-      <c r="V25" s="64"/>
-      <c r="W25" s="62"/>
+      <c r="U25" s="61"/>
+      <c r="V25" s="62"/>
+      <c r="W25" s="60"/>
       <c r="X25" s="1"/>
       <c r="Y25" s="7"/>
     </row>
     <row r="26" spans="1:25" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="73" t="s">
+      <c r="A26" s="70" t="s">
         <v>28</v>
       </c>
       <c r="B26" s="20" t="s">
@@ -3226,14 +3629,14 @@
       </c>
     </row>
     <row r="27" spans="1:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="69" t="s">
+      <c r="A27" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="97" t="s">
+      <c r="B27" s="96" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="98"/>
-      <c r="D27" s="99"/>
+      <c r="C27" s="97"/>
+      <c r="D27" s="98"/>
       <c r="E27" s="36"/>
       <c r="G27" s="8"/>
       <c r="H27" s="3"/>
@@ -3252,14 +3655,14 @@
       <c r="Y27" s="9"/>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A28" s="69" t="s">
+      <c r="A28" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="97" t="s">
+      <c r="B28" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="98"/>
-      <c r="D28" s="99"/>
+      <c r="C28" s="97"/>
+      <c r="D28" s="98"/>
       <c r="E28" s="36"/>
       <c r="G28" s="8"/>
       <c r="H28" s="3"/>
@@ -3278,10 +3681,10 @@
       <c r="Y28" s="9"/>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A29" s="69"/>
-      <c r="B29" s="97"/>
-      <c r="C29" s="98"/>
-      <c r="D29" s="99"/>
+      <c r="A29" s="67"/>
+      <c r="B29" s="96"/>
+      <c r="C29" s="97"/>
+      <c r="D29" s="98"/>
       <c r="E29" s="36"/>
       <c r="G29" s="8"/>
       <c r="H29" s="3"/>
@@ -3323,9 +3726,9 @@
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="32"/>
-      <c r="B31" s="100"/>
-      <c r="C31" s="101"/>
-      <c r="D31" s="102"/>
+      <c r="B31" s="90"/>
+      <c r="C31" s="91"/>
+      <c r="D31" s="92"/>
       <c r="E31" s="36"/>
       <c r="G31" s="8"/>
       <c r="H31" s="3"/>
@@ -3345,9 +3748,9 @@
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="32"/>
-      <c r="B32" s="100"/>
-      <c r="C32" s="101"/>
-      <c r="D32" s="102"/>
+      <c r="B32" s="90"/>
+      <c r="C32" s="91"/>
+      <c r="D32" s="92"/>
       <c r="E32" s="36"/>
       <c r="G32" s="8"/>
       <c r="H32" s="3"/>
@@ -3367,9 +3770,9 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" s="32"/>
-      <c r="B33" s="100"/>
-      <c r="C33" s="101"/>
-      <c r="D33" s="102"/>
+      <c r="B33" s="90"/>
+      <c r="C33" s="91"/>
+      <c r="D33" s="92"/>
       <c r="E33" s="36"/>
       <c r="G33" s="8"/>
       <c r="H33" s="3"/>
@@ -3389,9 +3792,9 @@
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="32"/>
-      <c r="B34" s="100"/>
-      <c r="C34" s="101"/>
-      <c r="D34" s="102"/>
+      <c r="B34" s="90"/>
+      <c r="C34" s="91"/>
+      <c r="D34" s="92"/>
       <c r="E34" s="36"/>
       <c r="G34" s="8"/>
       <c r="H34" s="3"/>
@@ -3411,9 +3814,9 @@
     </row>
     <row r="35" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="33"/>
-      <c r="B35" s="103"/>
-      <c r="C35" s="104"/>
-      <c r="D35" s="105"/>
+      <c r="B35" s="93"/>
+      <c r="C35" s="94"/>
+      <c r="D35" s="95"/>
       <c r="E35" s="37"/>
       <c r="G35" s="10"/>
       <c r="H35" s="11"/>
@@ -3435,10 +3838,15 @@
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0"/>
   <protectedRanges>
-    <protectedRange sqref="A24:H24 A12:P23 Q12:X24 A11:X11 V10:X10 A10:T10 A8:X9 A7:Y7 A6:X6 J24:P24" name="Contact Fields"/>
+    <protectedRange sqref="A24:B24 A12:B12 Q12:X24 A11:B11 V10:X10 A10:B10 A8:B8 A7:B7 A6:B6 J24:P24 D6:X6 D24:H24 A23:B23 D23:P23 A22:B22 D22:P22 A21:B21 D21:P21 A20:B20 D20:P20 A19:B19 D19:P19 A18:B18 D18:P18 A17:B17 D17:P17 A16:B16 D16:P16 A15:B15 D15:P15 A14:B14 D14:P14 A13:B13 D13:P13 D12:P12 D11:X11 D10:T10 A9:B9 D9:X9 D8:X8 D7:Y7" name="Contact Fields"/>
     <protectedRange sqref="A27:Y35 I24" name="Questionnaire"/>
   </protectedRanges>
   <mergeCells count="13">
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="W3:Y3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="O3:Q3"/>
     <mergeCell ref="B33:D33"/>
     <mergeCell ref="B34:D34"/>
     <mergeCell ref="B35:D35"/>
@@ -3447,122 +3855,269 @@
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="B32:D32"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="W3:Y3"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="O3:Q3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A25:AG25 A24:H24 B12:P23 B7:F7 J7 Q15:AG24 N7:R7 Q12:R14 V12:AG14 B8:AG11 U6:U7 V7 Z7:AG7 J24:P24">
-    <cfRule type="expression" dxfId="25" priority="47">
+  <conditionalFormatting sqref="A25:AG25 A24:B24 J7 Q15:AG24 N7:R7 V12:AG14 U6:U7 V7 Z7:AG7 J24:P24 D24:H24 D15:P23 D12:R14 B7:B23 D8:AG11 D7:F7">
+    <cfRule type="expression" dxfId="65" priority="87">
       <formula>$C6="x"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="48">
+    <cfRule type="expression" dxfId="64" priority="88">
       <formula>$D6="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W27:Y35 S27:U35 O27:Q35 K27:M35 G27:I35">
-    <cfRule type="expression" dxfId="23" priority="45">
+    <cfRule type="expression" dxfId="63" priority="85">
       <formula>$C27="x"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="46">
+    <cfRule type="expression" dxfId="62" priority="86">
       <formula>$D27="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:A23">
-    <cfRule type="expression" dxfId="21" priority="35">
+    <cfRule type="expression" dxfId="61" priority="75">
       <formula>$C7="x"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="36">
+    <cfRule type="expression" dxfId="60" priority="76">
       <formula>$D7="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24">
-    <cfRule type="expression" dxfId="19" priority="29">
+    <cfRule type="expression" dxfId="59" priority="69">
       <formula>$C24="x"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="30">
+    <cfRule type="expression" dxfId="58" priority="70">
       <formula>$D24="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:I7">
-    <cfRule type="expression" dxfId="17" priority="27">
+    <cfRule type="expression" dxfId="57" priority="67">
       <formula>$C6="x"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="28">
+    <cfRule type="expression" dxfId="56" priority="68">
       <formula>$D6="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:I7">
-    <cfRule type="expression" dxfId="15" priority="51">
+    <cfRule type="expression" dxfId="55" priority="91">
       <formula>$C12="x"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="52">
+    <cfRule type="expression" dxfId="54" priority="92">
       <formula>$D12="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S12:U12">
-    <cfRule type="expression" dxfId="13" priority="21">
+    <cfRule type="expression" dxfId="53" priority="61">
       <formula>$C12="x"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="22">
+    <cfRule type="expression" dxfId="52" priority="62">
       <formula>$D12="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S13:U14">
-    <cfRule type="expression" dxfId="11" priority="13">
+    <cfRule type="expression" dxfId="51" priority="53">
       <formula>$C13="x"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="14">
+    <cfRule type="expression" dxfId="50" priority="54">
       <formula>$D13="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S6:T7">
-    <cfRule type="expression" dxfId="9" priority="11">
+    <cfRule type="expression" dxfId="49" priority="51">
       <formula>$C6="x"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="12">
+    <cfRule type="expression" dxfId="48" priority="52">
       <formula>$D6="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W7:Y7">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="47" priority="47">
       <formula>$C7="x"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="46" priority="48">
       <formula>$D7="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7:M7">
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="45" priority="43">
       <formula>$C7="x"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="44" priority="44">
       <formula>$D7="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7:M7">
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="43" priority="45">
       <formula>$C12="x"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="42" priority="46">
       <formula>$D12="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:M6">
+    <cfRule type="expression" dxfId="41" priority="41">
+      <formula>$C6="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="42">
+      <formula>$D6="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="expression" dxfId="39" priority="39">
+      <formula>$C6="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="40">
+      <formula>$D6="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23">
+    <cfRule type="expression" dxfId="35" priority="35">
+      <formula>$C23="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="36">
+      <formula>$D23="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
+    <cfRule type="expression" dxfId="33" priority="33">
+      <formula>$C22="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="34">
+      <formula>$D22="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
+    <cfRule type="expression" dxfId="31" priority="31">
+      <formula>$C21="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="32">
+      <formula>$D21="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="expression" dxfId="29" priority="29">
+      <formula>$C20="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="30">
+      <formula>$D20="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="expression" dxfId="27" priority="27">
+      <formula>$C19="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="28">
+      <formula>$D19="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18">
+    <cfRule type="expression" dxfId="25" priority="25">
+      <formula>$C18="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="26">
+      <formula>$D18="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17">
+    <cfRule type="expression" dxfId="23" priority="23">
+      <formula>$C17="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="24">
+      <formula>$D17="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16">
+    <cfRule type="expression" dxfId="21" priority="21">
+      <formula>$C16="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="22">
+      <formula>$D16="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="expression" dxfId="19" priority="19">
+      <formula>$C15="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="20">
+      <formula>$D15="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="expression" dxfId="17" priority="17">
+      <formula>$C14="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="18">
+      <formula>$D14="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="expression" dxfId="15" priority="15">
+      <formula>$C13="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="16">
+      <formula>$D13="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="expression" dxfId="13" priority="13">
+      <formula>$C12="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="14">
+      <formula>$D12="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="expression" dxfId="11" priority="11">
+      <formula>$C11="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="12">
+      <formula>$D11="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="expression" dxfId="9" priority="9">
+      <formula>$C10="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="10">
+      <formula>$D10="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="expression" dxfId="7" priority="7">
+      <formula>$C9="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="8">
+      <formula>$D9="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="expression" dxfId="5" priority="5">
+      <formula>$C8="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="6">
+      <formula>$D8="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>$C7="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>$D7="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
     <cfRule type="expression" dxfId="1" priority="1">
-      <formula>$C6="x"</formula>
+      <formula>$C24="x"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>$D6="x"</formula>
+      <formula>$D24="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7" xr:uid="{800895DA-5639-438C-B977-CBBACBEDFF96}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:D7 C6 C8:C24" xr:uid="{800895DA-5639-438C-B977-CBBACBEDFF96}">
       <formula1>"x"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C24 D6 D8:D24" xr:uid="{25196C70-295C-43FF-A050-7D2EA327A7B4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:D24 D6" xr:uid="{25196C70-295C-43FF-A050-7D2EA327A7B4}">
       <formula1>#REF!</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:XFD1" xr:uid="{1CF26B28-1967-426C-8B8F-6D82F1D1CF4B}">
@@ -3579,6 +4134,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010060A44420B6B801499790497461B7617A" ma:contentTypeVersion="11" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="fabbcee23a04d27af1ae9e54f4461bef">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8f774076-1ef3-4740-8929-5969f04599b3" xmlns:ns4="8b2a92f5-6e7f-40fd-b6fe-382c9779cf32" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c03e0335abb4116b770311e5abaeb524" ns3:_="" ns4:_="">
     <xsd:import namespace="8f774076-1ef3-4740-8929-5969f04599b3"/>
@@ -3787,22 +4357,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDAAE1C4-DB1B-4159-B8B9-55C0242E8521}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="8b2a92f5-6e7f-40fd-b6fe-382c9779cf32"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="8f774076-1ef3-4740-8929-5969f04599b3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B94D2B0B-0398-4829-B93A-C49C0FAED7B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4CDBC7-0A6E-420D-A4CD-91BDFDE80302}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3819,29 +4399,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B94D2B0B-0398-4829-B93A-C49C0FAED7B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDAAE1C4-DB1B-4159-B8B9-55C0242E8521}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="8b2a92f5-6e7f-40fd-b6fe-382c9779cf32"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="8f774076-1ef3-4740-8929-5969f04599b3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>